<commit_message>
Uniform searches with LGA and VIcPol hierarchy
</commit_message>
<xml_diff>
--- a/Data/Police.station.location.xlsx
+++ b/Data/Police.station.location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monika/Documents/vicpoldata/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E248DC-21F5-5143-B929-8576548B4F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC9075E-32ED-CD4E-B973-C2925AF69FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-66040" yWindow="520" windowWidth="21800" windowHeight="12700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-63780" yWindow="-1080" windowWidth="21800" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="745">
   <si>
     <t>Station</t>
   </si>
@@ -571,9 +571,6 @@
     <t>ALEXANDRA</t>
   </si>
   <si>
-    <t>ALTONA NORTH POLICE STATION</t>
-  </si>
-  <si>
     <t>ALTONA NORTH</t>
   </si>
   <si>
@@ -670,9 +667,6 @@
     <t>FALLS CREEK POLICE STATION</t>
   </si>
   <si>
-    <t>Unincorporated Land (victoria)</t>
-  </si>
-  <si>
     <t>FALLS CREEK</t>
   </si>
   <si>
@@ -1441,9 +1435,6 @@
     <t>MELBOURNE AIRPORT</t>
   </si>
   <si>
-    <t>AFP - VIC AVIATION - MELBOURNE AIRPORT</t>
-  </si>
-  <si>
     <t>MELTON POLICE STATION</t>
   </si>
   <si>
@@ -1891,9 +1882,6 @@
     <t>ST ARNAUD</t>
   </si>
   <si>
-    <t>ST KILDA POLICE STATION</t>
-  </si>
-  <si>
     <t>ST KILDA</t>
   </si>
   <si>
@@ -2261,6 +2249,12 @@
   </si>
   <si>
     <t>WILSONS PROMONTORY</t>
+  </si>
+  <si>
+    <t>ALTONA POLICE STATION</t>
+  </si>
+  <si>
+    <t>ST. KILDA POLICE STATION</t>
   </si>
 </sst>
 </file>
@@ -2647,10 +2641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D333"/>
+  <dimension ref="A1:D332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
+      <selection activeCell="A272" sqref="A272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3598,13 +3592,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>183</v>
+        <v>743</v>
       </c>
       <c r="B68" t="s">
         <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D68">
         <v>3025</v>
@@ -3612,13 +3606,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B69" t="s">
         <v>119</v>
       </c>
       <c r="C69" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D69">
         <v>3230</v>
@@ -3626,13 +3620,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B70" t="s">
         <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D70">
         <v>3233</v>
@@ -3640,13 +3634,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B71" t="s">
         <v>57</v>
       </c>
       <c r="C71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D71">
         <v>3319</v>
@@ -3654,13 +3648,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B72" t="s">
         <v>40</v>
       </c>
       <c r="C72" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D72">
         <v>3377</v>
@@ -3668,13 +3662,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>192</v>
+      </c>
+      <c r="B73" t="s">
         <v>193</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>194</v>
-      </c>
-      <c r="C73" t="s">
-        <v>195</v>
       </c>
       <c r="D73">
         <v>3147</v>
@@ -3682,13 +3676,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B74" t="s">
         <v>101</v>
       </c>
       <c r="C74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D74">
         <v>3467</v>
@@ -3696,13 +3690,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B75" t="s">
         <v>19</v>
       </c>
       <c r="C75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D75">
         <v>3034</v>
@@ -3710,13 +3704,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B76" t="s">
         <v>92</v>
       </c>
       <c r="C76" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D76">
         <v>3551</v>
@@ -3724,13 +3718,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>201</v>
+      </c>
+      <c r="B77" t="s">
         <v>202</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>203</v>
-      </c>
-      <c r="C77" t="s">
-        <v>204</v>
       </c>
       <c r="D77">
         <v>3340</v>
@@ -3738,13 +3732,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B78" t="s">
         <v>139</v>
       </c>
       <c r="C78" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D78">
         <v>3875</v>
@@ -3752,13 +3746,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>206</v>
+      </c>
+      <c r="B79" t="s">
+        <v>202</v>
+      </c>
+      <c r="C79" t="s">
         <v>207</v>
-      </c>
-      <c r="B79" t="s">
-        <v>203</v>
-      </c>
-      <c r="C79" t="s">
-        <v>208</v>
       </c>
       <c r="D79">
         <v>3342</v>
@@ -3766,13 +3760,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B80" t="s">
         <v>31</v>
       </c>
       <c r="C80" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D80">
         <v>3350</v>
@@ -3780,13 +3774,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B81" t="s">
         <v>14</v>
       </c>
       <c r="C81" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D81">
         <v>3407</v>
@@ -3794,13 +3788,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B82" t="s">
         <v>113</v>
       </c>
       <c r="C82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D82">
         <v>3666</v>
@@ -3808,13 +3802,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>214</v>
+      </c>
+      <c r="B83" t="s">
+        <v>48</v>
+      </c>
+      <c r="C83" t="s">
         <v>215</v>
-      </c>
-      <c r="B83" t="s">
-        <v>216</v>
-      </c>
-      <c r="C83" t="s">
-        <v>217</v>
       </c>
       <c r="D83">
         <v>3699</v>
@@ -3822,13 +3816,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B84" t="s">
         <v>178</v>
       </c>
       <c r="C84" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D84">
         <v>3065</v>
@@ -3836,13 +3830,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>218</v>
+      </c>
+      <c r="B85" t="s">
+        <v>219</v>
+      </c>
+      <c r="C85" t="s">
         <v>220</v>
-      </c>
-      <c r="B85" t="s">
-        <v>221</v>
-      </c>
-      <c r="C85" t="s">
-        <v>222</v>
       </c>
       <c r="D85">
         <v>3011</v>
@@ -3850,13 +3844,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
       </c>
       <c r="C86" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D86">
         <v>3236</v>
@@ -3864,13 +3858,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B87" t="s">
         <v>84</v>
       </c>
       <c r="C87" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D87">
         <v>3960</v>
@@ -3878,13 +3872,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>225</v>
+      </c>
+      <c r="B88" t="s">
+        <v>226</v>
+      </c>
+      <c r="C88" t="s">
         <v>227</v>
-      </c>
-      <c r="B88" t="s">
-        <v>228</v>
-      </c>
-      <c r="C88" t="s">
-        <v>229</v>
       </c>
       <c r="D88">
         <v>3199</v>
@@ -3892,13 +3886,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>228</v>
+      </c>
+      <c r="B89" t="s">
+        <v>229</v>
+      </c>
+      <c r="C89" t="s">
         <v>230</v>
-      </c>
-      <c r="B89" t="s">
-        <v>231</v>
-      </c>
-      <c r="C89" t="s">
-        <v>232</v>
       </c>
       <c r="D89">
         <v>3311</v>
@@ -3906,13 +3900,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>231</v>
+      </c>
+      <c r="B90" t="s">
+        <v>232</v>
+      </c>
+      <c r="C90" t="s">
         <v>233</v>
-      </c>
-      <c r="B90" t="s">
-        <v>234</v>
-      </c>
-      <c r="C90" t="s">
-        <v>235</v>
       </c>
       <c r="D90">
         <v>3450</v>
@@ -3920,13 +3914,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>234</v>
+      </c>
+      <c r="B91" t="s">
+        <v>235</v>
+      </c>
+      <c r="C91" t="s">
         <v>236</v>
-      </c>
-      <c r="B91" t="s">
-        <v>237</v>
-      </c>
-      <c r="C91" t="s">
-        <v>238</v>
       </c>
       <c r="D91">
         <v>3162</v>
@@ -3934,13 +3928,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B92" t="s">
         <v>14</v>
       </c>
       <c r="C92" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D92">
         <v>3314</v>
@@ -3948,13 +3942,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B93" t="s">
         <v>166</v>
       </c>
       <c r="C93" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D93">
         <v>3525</v>
@@ -3962,13 +3956,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B94" t="s">
         <v>22</v>
       </c>
       <c r="C94" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D94">
         <v>3196</v>
@@ -3976,13 +3970,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B95" t="s">
         <v>148</v>
       </c>
       <c r="C95" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D95">
         <v>3683</v>
@@ -3990,13 +3984,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B96" t="s">
         <v>79</v>
       </c>
       <c r="C96" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D96">
         <v>3842</v>
@@ -4004,13 +3998,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>247</v>
+      </c>
+      <c r="B97" t="s">
+        <v>248</v>
+      </c>
+      <c r="C97" t="s">
         <v>249</v>
-      </c>
-      <c r="B97" t="s">
-        <v>250</v>
-      </c>
-      <c r="C97" t="s">
-        <v>251</v>
       </c>
       <c r="D97">
         <v>3168</v>
@@ -4018,13 +4012,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B98" t="s">
         <v>25</v>
       </c>
       <c r="C98" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D98">
         <v>3370</v>
@@ -4032,13 +4026,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B99" t="s">
         <v>98</v>
       </c>
       <c r="C99" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D99">
         <v>3266</v>
@@ -4046,13 +4040,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>254</v>
+      </c>
+      <c r="B100" t="s">
+        <v>255</v>
+      </c>
+      <c r="C100" t="s">
         <v>256</v>
-      </c>
-      <c r="B100" t="s">
-        <v>257</v>
-      </c>
-      <c r="C100" t="s">
-        <v>258</v>
       </c>
       <c r="D100">
         <v>3644</v>
@@ -4060,13 +4054,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>257</v>
+      </c>
+      <c r="B101" t="s">
+        <v>258</v>
+      </c>
+      <c r="C101" t="s">
         <v>259</v>
-      </c>
-      <c r="B101" t="s">
-        <v>260</v>
-      </c>
-      <c r="C101" t="s">
-        <v>261</v>
       </c>
       <c r="D101">
         <v>3568</v>
@@ -4074,13 +4068,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B102" t="s">
         <v>14</v>
       </c>
       <c r="C102" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D102">
         <v>3315</v>
@@ -4088,13 +4082,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>262</v>
+      </c>
+      <c r="B103" t="s">
+        <v>263</v>
+      </c>
+      <c r="C103" t="s">
         <v>264</v>
-      </c>
-      <c r="B103" t="s">
-        <v>265</v>
-      </c>
-      <c r="C103" t="s">
-        <v>266</v>
       </c>
       <c r="D103">
         <v>3214</v>
@@ -4102,13 +4096,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B104" t="s">
         <v>161</v>
       </c>
       <c r="C104" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D104">
         <v>3707</v>
@@ -4116,13 +4110,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B105" t="s">
         <v>54</v>
       </c>
       <c r="C105" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D105">
         <v>3922</v>
@@ -4130,13 +4124,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B106" t="s">
         <v>133</v>
       </c>
       <c r="C106" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D106">
         <v>3064</v>
@@ -4144,13 +4138,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>271</v>
+      </c>
+      <c r="B107" t="s">
+        <v>272</v>
+      </c>
+      <c r="C107" t="s">
         <v>273</v>
-      </c>
-      <c r="B107" t="s">
-        <v>274</v>
-      </c>
-      <c r="C107" t="s">
-        <v>275</v>
       </c>
       <c r="D107">
         <v>3977</v>
@@ -4158,13 +4152,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>274</v>
+      </c>
+      <c r="B108" t="s">
+        <v>275</v>
+      </c>
+      <c r="C108" t="s">
         <v>276</v>
-      </c>
-      <c r="B108" t="s">
-        <v>277</v>
-      </c>
-      <c r="C108" t="s">
-        <v>278</v>
       </c>
       <c r="D108">
         <v>3136</v>
@@ -4172,13 +4166,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B109" t="s">
         <v>166</v>
       </c>
       <c r="C109" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D109">
         <v>3530</v>
@@ -4186,13 +4180,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>279</v>
+      </c>
+      <c r="B110" t="s">
+        <v>280</v>
+      </c>
+      <c r="C110" t="s">
         <v>281</v>
-      </c>
-      <c r="B110" t="s">
-        <v>282</v>
-      </c>
-      <c r="C110" t="s">
-        <v>283</v>
       </c>
       <c r="D110">
         <v>3175</v>
@@ -4200,13 +4194,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B111" t="s">
         <v>25</v>
       </c>
       <c r="C111" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D111">
         <v>3460</v>
@@ -4214,13 +4208,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B112" t="s">
         <v>48</v>
       </c>
       <c r="C112" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D112">
         <v>3691</v>
@@ -4228,13 +4222,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B113" t="s">
         <v>43</v>
       </c>
       <c r="C113" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D113">
         <v>3089</v>
@@ -4242,13 +4236,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B114" t="s">
         <v>74</v>
       </c>
       <c r="C114" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D114">
         <v>3008</v>
@@ -4256,13 +4250,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B115" t="s">
         <v>166</v>
       </c>
       <c r="C115" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D115">
         <v>3480</v>
@@ -4270,13 +4264,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>292</v>
+      </c>
+      <c r="B116" t="s">
+        <v>293</v>
+      </c>
+      <c r="C116" t="s">
         <v>294</v>
-      </c>
-      <c r="B116" t="s">
-        <v>295</v>
-      </c>
-      <c r="C116" t="s">
-        <v>296</v>
       </c>
       <c r="D116">
         <v>3109</v>
@@ -4284,13 +4278,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B117" t="s">
         <v>139</v>
       </c>
       <c r="C117" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D117">
         <v>3885</v>
@@ -4298,13 +4292,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B118" t="s">
         <v>8</v>
       </c>
       <c r="C118" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D118">
         <v>3815</v>
@@ -4312,13 +4306,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B119" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C119" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D119">
         <v>3124</v>
@@ -4326,13 +4320,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B120" t="s">
         <v>98</v>
       </c>
       <c r="C120" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D120">
         <v>3260</v>
@@ -4340,13 +4334,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B121" t="s">
         <v>139</v>
       </c>
       <c r="C121" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D121">
         <v>3890</v>
@@ -4354,13 +4348,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>305</v>
+      </c>
+      <c r="B122" t="s">
+        <v>306</v>
+      </c>
+      <c r="C122" t="s">
         <v>307</v>
-      </c>
-      <c r="B122" t="s">
-        <v>308</v>
-      </c>
-      <c r="C122" t="s">
-        <v>309</v>
       </c>
       <c r="D122">
         <v>3023</v>
@@ -4368,13 +4362,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B123" t="s">
         <v>87</v>
       </c>
       <c r="C123" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D123">
         <v>3646</v>
@@ -4382,13 +4376,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
+        <v>310</v>
+      </c>
+      <c r="B124" t="s">
+        <v>311</v>
+      </c>
+      <c r="C124" t="s">
         <v>312</v>
-      </c>
-      <c r="B124" t="s">
-        <v>313</v>
-      </c>
-      <c r="C124" t="s">
-        <v>314</v>
       </c>
       <c r="D124">
         <v>3936</v>
@@ -4396,13 +4390,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>313</v>
+      </c>
+      <c r="B125" t="s">
+        <v>314</v>
+      </c>
+      <c r="C125" t="s">
         <v>315</v>
-      </c>
-      <c r="B125" t="s">
-        <v>316</v>
-      </c>
-      <c r="C125" t="s">
-        <v>317</v>
       </c>
       <c r="D125">
         <v>3818</v>
@@ -4410,13 +4404,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B126" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C126" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D126">
         <v>3222</v>
@@ -4424,13 +4418,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B127" t="s">
         <v>14</v>
       </c>
       <c r="C127" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D127">
         <v>3294</v>
@@ -4438,13 +4432,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B128" t="s">
         <v>60</v>
       </c>
       <c r="C128" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D128">
         <v>3564</v>
@@ -4452,13 +4446,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B129" t="s">
         <v>57</v>
       </c>
       <c r="C129" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D129">
         <v>3318</v>
@@ -4466,13 +4460,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B130" t="s">
         <v>181</v>
       </c>
       <c r="C130" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D130">
         <v>3713</v>
@@ -4480,13 +4474,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B131" t="s">
         <v>92</v>
       </c>
       <c r="C131" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D131">
         <v>3558</v>
@@ -4494,13 +4488,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B132" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C132" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D132">
         <v>3802</v>
@@ -4508,13 +4502,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>330</v>
+      </c>
+      <c r="B133" t="s">
+        <v>331</v>
+      </c>
+      <c r="C133" t="s">
         <v>332</v>
-      </c>
-      <c r="B133" t="s">
-        <v>333</v>
-      </c>
-      <c r="C133" t="s">
-        <v>334</v>
       </c>
       <c r="D133">
         <v>3076</v>
@@ -4522,13 +4516,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B134" t="s">
         <v>19</v>
       </c>
       <c r="C134" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D134">
         <v>3041</v>
@@ -4536,13 +4530,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B135" t="s">
         <v>151</v>
       </c>
       <c r="C135" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D135">
         <v>3777</v>
@@ -4550,13 +4544,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B136" t="s">
         <v>92</v>
       </c>
       <c r="C136" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D136">
         <v>3523</v>
@@ -4564,13 +4558,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B137" t="s">
         <v>69</v>
       </c>
       <c r="C137" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D137">
         <v>3084</v>
@@ -4578,13 +4572,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B138" t="s">
         <v>122</v>
       </c>
       <c r="C138" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D138">
         <v>3858</v>
@@ -4592,13 +4586,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B139" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C139" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D139">
         <v>3304</v>
@@ -4606,13 +4600,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B140" t="s">
         <v>95</v>
       </c>
       <c r="C140" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D140">
         <v>3396</v>
@@ -4620,13 +4614,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>347</v>
+      </c>
+      <c r="B141" t="s">
+        <v>348</v>
+      </c>
+      <c r="C141" t="s">
         <v>349</v>
-      </c>
-      <c r="B141" t="s">
-        <v>350</v>
-      </c>
-      <c r="C141" t="s">
-        <v>351</v>
       </c>
       <c r="D141">
         <v>3400</v>
@@ -4634,13 +4628,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B142" t="s">
         <v>43</v>
       </c>
       <c r="C142" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D142">
         <v>3099</v>
@@ -4648,13 +4642,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B143" t="s">
         <v>125</v>
       </c>
       <c r="C143" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D143">
         <v>3517</v>
@@ -4662,13 +4656,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B144" t="s">
         <v>31</v>
       </c>
       <c r="C144" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D144">
         <v>3350</v>
@@ -4676,13 +4670,13 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
+        <v>356</v>
+      </c>
+      <c r="B145" t="s">
+        <v>357</v>
+      </c>
+      <c r="C145" t="s">
         <v>358</v>
-      </c>
-      <c r="B145" t="s">
-        <v>359</v>
-      </c>
-      <c r="C145" t="s">
-        <v>360</v>
       </c>
       <c r="D145">
         <v>3723</v>
@@ -4690,13 +4684,13 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B146" t="s">
         <v>28</v>
       </c>
       <c r="C146" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D146">
         <v>3423</v>
@@ -4704,13 +4698,13 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B147" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C147" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D147">
         <v>3649</v>
@@ -4718,13 +4712,13 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
+        <v>363</v>
+      </c>
+      <c r="B148" t="s">
+        <v>364</v>
+      </c>
+      <c r="C148" t="s">
         <v>365</v>
-      </c>
-      <c r="B148" t="s">
-        <v>366</v>
-      </c>
-      <c r="C148" t="s">
-        <v>367</v>
       </c>
       <c r="D148">
         <v>3038</v>
@@ -4732,13 +4726,13 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B149" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C149" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D149">
         <v>3579</v>
@@ -4746,13 +4740,13 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B150" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C150" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D150">
         <v>3101</v>
@@ -4760,13 +4754,13 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B151" t="s">
         <v>130</v>
       </c>
       <c r="C151" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D151">
         <v>3764</v>
@@ -4774,13 +4768,13 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B152" t="s">
         <v>181</v>
       </c>
       <c r="C152" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D152">
         <v>3763</v>
@@ -4788,13 +4782,13 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B153" t="s">
         <v>8</v>
       </c>
       <c r="C153" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D153">
         <v>3981</v>
@@ -4802,13 +4796,13 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B154" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C154" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D154">
         <v>3580</v>
@@ -4816,13 +4810,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>378</v>
+      </c>
+      <c r="B155" t="s">
+        <v>379</v>
+      </c>
+      <c r="C155" t="s">
         <v>380</v>
-      </c>
-      <c r="B155" t="s">
-        <v>381</v>
-      </c>
-      <c r="C155" t="s">
-        <v>382</v>
       </c>
       <c r="D155">
         <v>3282</v>
@@ -4830,13 +4824,13 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B156" t="s">
         <v>84</v>
       </c>
       <c r="C156" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D156">
         <v>3950</v>
@@ -4844,13 +4838,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B157" t="s">
         <v>11</v>
       </c>
       <c r="C157" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D157">
         <v>3444</v>
@@ -4858,13 +4852,13 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>385</v>
+      </c>
+      <c r="B158" t="s">
+        <v>386</v>
+      </c>
+      <c r="C158" t="s">
         <v>387</v>
-      </c>
-      <c r="B158" t="s">
-        <v>388</v>
-      </c>
-      <c r="C158" t="s">
-        <v>389</v>
       </c>
       <c r="D158">
         <v>3584</v>
@@ -4872,13 +4866,13 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B159" t="s">
         <v>40</v>
       </c>
       <c r="C159" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D159">
         <v>3351</v>
@@ -4886,13 +4880,13 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B160" t="s">
         <v>139</v>
       </c>
       <c r="C160" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D160">
         <v>3909</v>
@@ -4900,13 +4894,13 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B161" t="s">
         <v>11</v>
       </c>
       <c r="C161" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D161">
         <v>3435</v>
@@ -4914,13 +4908,13 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B162" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C162" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D162">
         <v>3200</v>
@@ -4928,13 +4922,13 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B163" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C163" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D163">
         <v>3220</v>
@@ -4942,13 +4936,13 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B164" t="s">
         <v>11</v>
       </c>
       <c r="C164" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D164">
         <v>3437</v>
@@ -4956,13 +4950,13 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B165" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C165" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D165">
         <v>3150</v>
@@ -4970,13 +4964,13 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B166" t="s">
         <v>92</v>
       </c>
       <c r="C166" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D166">
         <v>3557</v>
@@ -4984,13 +4978,13 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B167" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C167" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D167">
         <v>3345</v>
@@ -4998,13 +4992,13 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B168" t="s">
         <v>57</v>
       </c>
       <c r="C168" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D168">
         <v>3412</v>
@@ -5012,13 +5006,13 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B169" t="s">
         <v>101</v>
       </c>
       <c r="C169" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D169">
         <v>3384</v>
@@ -5026,13 +5020,13 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B170" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C170" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D170">
         <v>3212</v>
@@ -5040,13 +5034,13 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B171" t="s">
         <v>5</v>
       </c>
       <c r="C171" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D171">
         <v>3238</v>
@@ -5054,13 +5048,13 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B172" t="s">
         <v>31</v>
       </c>
       <c r="C172" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D172">
         <v>3352</v>
@@ -5068,13 +5062,13 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B173" t="s">
         <v>84</v>
       </c>
       <c r="C173" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D173">
         <v>3953</v>
@@ -5082,13 +5076,13 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B174" t="s">
         <v>101</v>
       </c>
       <c r="C174" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D174">
         <v>3352</v>
@@ -5096,13 +5090,13 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B175" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C175" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D175">
         <v>3216</v>
@@ -5110,13 +5104,13 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B176" t="s">
         <v>60</v>
       </c>
       <c r="C176" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D176">
         <v>3566</v>
@@ -5124,13 +5118,13 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B177" t="s">
         <v>136</v>
       </c>
       <c r="C177" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D177">
         <v>3046</v>
@@ -5138,13 +5132,13 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
+        <v>426</v>
+      </c>
+      <c r="B178" t="s">
+        <v>427</v>
+      </c>
+      <c r="C178" t="s">
         <v>428</v>
-      </c>
-      <c r="B178" t="s">
-        <v>429</v>
-      </c>
-      <c r="C178" t="s">
-        <v>430</v>
       </c>
       <c r="D178">
         <v>3381</v>
@@ -5152,13 +5146,13 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B179" t="s">
         <v>14</v>
       </c>
       <c r="C179" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D179">
         <v>3300</v>
@@ -5166,13 +5160,13 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B180" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C180" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D180">
         <v>3915</v>
@@ -5180,13 +5174,13 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B181" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C181" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D181">
         <v>3462</v>
@@ -5194,13 +5188,13 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B182" t="s">
         <v>28</v>
       </c>
       <c r="C182" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D182">
         <v>3418</v>
@@ -5208,13 +5202,13 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B183" t="s">
         <v>74</v>
       </c>
       <c r="C183" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D183">
         <v>3051</v>
@@ -5222,13 +5216,13 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
+        <v>439</v>
+      </c>
+      <c r="B184" t="s">
+        <v>440</v>
+      </c>
+      <c r="C184" t="s">
         <v>441</v>
-      </c>
-      <c r="B184" t="s">
-        <v>442</v>
-      </c>
-      <c r="C184" t="s">
-        <v>443</v>
       </c>
       <c r="D184">
         <v>3070</v>
@@ -5236,13 +5230,13 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B185" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C185" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D185">
         <v>3636</v>
@@ -5250,13 +5244,13 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B186" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C186" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D186">
         <v>3594</v>
@@ -5264,13 +5258,13 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B187" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C187" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D187">
         <v>3166</v>
@@ -5278,13 +5272,13 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B188" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C188" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D188">
         <v>3226</v>
@@ -5292,13 +5286,13 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B189" t="s">
         <v>122</v>
       </c>
       <c r="C189" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D189">
         <v>3860</v>
@@ -5306,13 +5300,13 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B190" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C190" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D190">
         <v>3463</v>
@@ -5320,13 +5314,13 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B191" t="s">
         <v>139</v>
       </c>
       <c r="C191" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D191">
         <v>3892</v>
@@ -5334,13 +5328,13 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
+        <v>456</v>
+      </c>
+      <c r="B192" t="s">
+        <v>457</v>
+      </c>
+      <c r="C192" t="s">
         <v>458</v>
-      </c>
-      <c r="B192" t="s">
-        <v>459</v>
-      </c>
-      <c r="C192" t="s">
-        <v>460</v>
       </c>
       <c r="D192">
         <v>3144</v>
@@ -5348,13 +5342,13 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B193" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C193" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D193">
         <v>3546</v>
@@ -5362,13 +5356,13 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B194" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C194" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D194">
         <v>3722</v>
@@ -5376,13 +5370,13 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B195" t="s">
         <v>37</v>
       </c>
       <c r="C195" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D195">
         <v>3465</v>
@@ -5390,13 +5384,13 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B196" t="s">
         <v>181</v>
       </c>
       <c r="C196" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D196">
         <v>3779</v>
@@ -5404,13 +5398,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B197" t="s">
         <v>84</v>
       </c>
       <c r="C197" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D197">
         <v>3956</v>
@@ -5418,13 +5412,13 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B198" t="s">
         <v>133</v>
       </c>
       <c r="C198" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D198">
         <v>3045</v>
@@ -5432,30 +5426,30 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B199" t="s">
-        <v>133</v>
+        <v>306</v>
       </c>
       <c r="C199" t="s">
         <v>472</v>
       </c>
       <c r="D199">
-        <v>3045</v>
+        <v>3337</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
+        <v>473</v>
+      </c>
+      <c r="B200" t="s">
         <v>474</v>
-      </c>
-      <c r="B200" t="s">
-        <v>308</v>
       </c>
       <c r="C200" t="s">
         <v>475</v>
       </c>
       <c r="D200">
-        <v>3337</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -5463,503 +5457,503 @@
         <v>476</v>
       </c>
       <c r="B201" t="s">
+        <v>229</v>
+      </c>
+      <c r="C201" t="s">
         <v>477</v>
       </c>
-      <c r="C201" t="s">
-        <v>478</v>
-      </c>
       <c r="D201">
-        <v>3505</v>
+        <v>3310</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>478</v>
+      </c>
+      <c r="B202" t="s">
+        <v>331</v>
+      </c>
+      <c r="C202" t="s">
         <v>479</v>
       </c>
-      <c r="B202" t="s">
-        <v>231</v>
-      </c>
-      <c r="C202" t="s">
-        <v>480</v>
-      </c>
       <c r="D202">
-        <v>3310</v>
+        <v>3754</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
+        <v>480</v>
+      </c>
+      <c r="B203" t="s">
+        <v>474</v>
+      </c>
+      <c r="C203" t="s">
         <v>481</v>
       </c>
-      <c r="B203" t="s">
-        <v>333</v>
-      </c>
-      <c r="C203" t="s">
-        <v>482</v>
-      </c>
       <c r="D203">
-        <v>3754</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
+        <v>482</v>
+      </c>
+      <c r="B204" t="s">
+        <v>331</v>
+      </c>
+      <c r="C204" t="s">
         <v>483</v>
       </c>
-      <c r="B204" t="s">
-        <v>477</v>
-      </c>
-      <c r="C204" t="s">
-        <v>484</v>
-      </c>
       <c r="D204">
-        <v>3500</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
+        <v>484</v>
+      </c>
+      <c r="B205" t="s">
+        <v>95</v>
+      </c>
+      <c r="C205" t="s">
         <v>485</v>
       </c>
-      <c r="B205" t="s">
-        <v>333</v>
-      </c>
-      <c r="C205" t="s">
-        <v>486</v>
-      </c>
       <c r="D205">
-        <v>3082</v>
+        <v>3392</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
+        <v>486</v>
+      </c>
+      <c r="B206" t="s">
+        <v>84</v>
+      </c>
+      <c r="C206" t="s">
         <v>487</v>
       </c>
-      <c r="B206" t="s">
-        <v>95</v>
-      </c>
-      <c r="C206" t="s">
-        <v>488</v>
-      </c>
       <c r="D206">
-        <v>3392</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
+        <v>488</v>
+      </c>
+      <c r="B207" t="s">
+        <v>161</v>
+      </c>
+      <c r="C207" t="s">
         <v>489</v>
       </c>
-      <c r="B207" t="s">
-        <v>84</v>
-      </c>
-      <c r="C207" t="s">
-        <v>490</v>
-      </c>
       <c r="D207">
-        <v>3871</v>
+        <v>3701</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
+        <v>490</v>
+      </c>
+      <c r="B208" t="s">
+        <v>151</v>
+      </c>
+      <c r="C208" t="s">
         <v>491</v>
       </c>
-      <c r="B208" t="s">
-        <v>161</v>
-      </c>
-      <c r="C208" t="s">
-        <v>492</v>
-      </c>
       <c r="D208">
-        <v>3701</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
+        <v>492</v>
+      </c>
+      <c r="B209" t="s">
+        <v>19</v>
+      </c>
+      <c r="C209" t="s">
         <v>493</v>
       </c>
-      <c r="B209" t="s">
-        <v>151</v>
-      </c>
-      <c r="C209" t="s">
-        <v>494</v>
-      </c>
       <c r="D209">
-        <v>3793</v>
+        <v>3039</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
+        <v>494</v>
+      </c>
+      <c r="B210" t="s">
+        <v>22</v>
+      </c>
+      <c r="C210" t="s">
         <v>495</v>
       </c>
-      <c r="B210" t="s">
-        <v>19</v>
-      </c>
-      <c r="C210" t="s">
-        <v>496</v>
-      </c>
       <c r="D210">
-        <v>3039</v>
+        <v>3189</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
+        <v>496</v>
+      </c>
+      <c r="B211" t="s">
+        <v>151</v>
+      </c>
+      <c r="C211" t="s">
         <v>497</v>
       </c>
-      <c r="B211" t="s">
-        <v>22</v>
-      </c>
-      <c r="C211" t="s">
-        <v>498</v>
-      </c>
       <c r="D211">
-        <v>3189</v>
+        <v>3138</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
+        <v>498</v>
+      </c>
+      <c r="B212" t="s">
+        <v>87</v>
+      </c>
+      <c r="C212" t="s">
         <v>499</v>
       </c>
-      <c r="B212" t="s">
-        <v>151</v>
-      </c>
-      <c r="C212" t="s">
-        <v>500</v>
-      </c>
       <c r="D212">
-        <v>3138</v>
+        <v>3629</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
+        <v>500</v>
+      </c>
+      <c r="B213" t="s">
+        <v>22</v>
+      </c>
+      <c r="C213" t="s">
         <v>501</v>
       </c>
-      <c r="B213" t="s">
-        <v>87</v>
-      </c>
-      <c r="C213" t="s">
-        <v>502</v>
-      </c>
       <c r="D213">
-        <v>3629</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
+        <v>502</v>
+      </c>
+      <c r="B214" t="s">
+        <v>311</v>
+      </c>
+      <c r="C214" t="s">
         <v>503</v>
       </c>
-      <c r="B214" t="s">
-        <v>22</v>
-      </c>
-      <c r="C214" t="s">
-        <v>504</v>
-      </c>
       <c r="D214">
-        <v>3195</v>
+        <v>3931</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
+        <v>504</v>
+      </c>
+      <c r="B215" t="s">
+        <v>151</v>
+      </c>
+      <c r="C215" t="s">
         <v>505</v>
       </c>
-      <c r="B215" t="s">
-        <v>313</v>
-      </c>
-      <c r="C215" t="s">
-        <v>506</v>
-      </c>
       <c r="D215">
-        <v>3931</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
+        <v>506</v>
+      </c>
+      <c r="B216" t="s">
+        <v>98</v>
+      </c>
+      <c r="C216" t="s">
         <v>507</v>
       </c>
-      <c r="B216" t="s">
-        <v>151</v>
-      </c>
-      <c r="C216" t="s">
-        <v>508</v>
-      </c>
       <c r="D216">
-        <v>3140</v>
+        <v>3324</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
+        <v>508</v>
+      </c>
+      <c r="B217" t="s">
+        <v>122</v>
+      </c>
+      <c r="C217" t="s">
         <v>509</v>
       </c>
-      <c r="B217" t="s">
-        <v>98</v>
-      </c>
-      <c r="C217" t="s">
-        <v>510</v>
-      </c>
       <c r="D217">
-        <v>3324</v>
+        <v>3851</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
+        <v>510</v>
+      </c>
+      <c r="B218" t="s">
+        <v>119</v>
+      </c>
+      <c r="C218" t="s">
         <v>511</v>
       </c>
-      <c r="B218" t="s">
-        <v>122</v>
-      </c>
-      <c r="C218" t="s">
-        <v>512</v>
-      </c>
       <c r="D218">
-        <v>3851</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
+        <v>512</v>
+      </c>
+      <c r="B219" t="s">
+        <v>379</v>
+      </c>
+      <c r="C219" t="s">
         <v>513</v>
       </c>
-      <c r="B219" t="s">
-        <v>119</v>
-      </c>
-      <c r="C219" t="s">
-        <v>514</v>
-      </c>
       <c r="D219">
-        <v>3232</v>
+        <v>3286</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
+        <v>514</v>
+      </c>
+      <c r="B220" t="s">
+        <v>11</v>
+      </c>
+      <c r="C220" t="s">
         <v>515</v>
       </c>
-      <c r="B220" t="s">
-        <v>381</v>
-      </c>
-      <c r="C220" t="s">
-        <v>516</v>
-      </c>
       <c r="D220">
-        <v>3286</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
+        <v>516</v>
+      </c>
+      <c r="B221" t="s">
+        <v>379</v>
+      </c>
+      <c r="C221" t="s">
         <v>517</v>
       </c>
-      <c r="B221" t="s">
-        <v>11</v>
-      </c>
-      <c r="C221" t="s">
-        <v>518</v>
-      </c>
       <c r="D221">
-        <v>3440</v>
+        <v>3272</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
+        <v>518</v>
+      </c>
+      <c r="B222" t="s">
+        <v>79</v>
+      </c>
+      <c r="C222" t="s">
         <v>519</v>
       </c>
-      <c r="B222" t="s">
-        <v>381</v>
-      </c>
-      <c r="C222" t="s">
-        <v>520</v>
-      </c>
       <c r="D222">
-        <v>3272</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
+        <v>520</v>
+      </c>
+      <c r="B223" t="s">
+        <v>48</v>
+      </c>
+      <c r="C223" t="s">
         <v>521</v>
       </c>
-      <c r="B223" t="s">
-        <v>79</v>
-      </c>
-      <c r="C223" t="s">
-        <v>522</v>
-      </c>
       <c r="D223">
-        <v>3840</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
+        <v>522</v>
+      </c>
+      <c r="B224" t="s">
+        <v>357</v>
+      </c>
+      <c r="C224" t="s">
         <v>523</v>
       </c>
-      <c r="B224" t="s">
-        <v>48</v>
-      </c>
-      <c r="C224" t="s">
-        <v>524</v>
-      </c>
       <c r="D224">
-        <v>3699</v>
+        <v>3723</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
+        <v>524</v>
+      </c>
+      <c r="B225" t="s">
+        <v>151</v>
+      </c>
+      <c r="C225" t="s">
         <v>525</v>
       </c>
-      <c r="B225" t="s">
-        <v>216</v>
-      </c>
-      <c r="C225" t="s">
-        <v>526</v>
-      </c>
       <c r="D225">
-        <v>3723</v>
+        <v>3796</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
+        <v>526</v>
+      </c>
+      <c r="B226" t="s">
+        <v>248</v>
+      </c>
+      <c r="C226" t="s">
         <v>527</v>
       </c>
-      <c r="B226" t="s">
-        <v>151</v>
-      </c>
-      <c r="C226" t="s">
-        <v>528</v>
-      </c>
       <c r="D226">
-        <v>3796</v>
+        <v>3149</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
+        <v>528</v>
+      </c>
+      <c r="B227" t="s">
+        <v>63</v>
+      </c>
+      <c r="C227" t="s">
         <v>529</v>
       </c>
-      <c r="B227" t="s">
-        <v>250</v>
-      </c>
-      <c r="C227" t="s">
-        <v>530</v>
-      </c>
       <c r="D227">
-        <v>3149</v>
+        <v>3732</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
+        <v>530</v>
+      </c>
+      <c r="B228" t="s">
+        <v>474</v>
+      </c>
+      <c r="C228" t="s">
         <v>531</v>
       </c>
-      <c r="B228" t="s">
-        <v>63</v>
-      </c>
-      <c r="C228" t="s">
-        <v>532</v>
-      </c>
       <c r="D228">
-        <v>3732</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
+        <v>532</v>
+      </c>
+      <c r="B229" t="s">
+        <v>95</v>
+      </c>
+      <c r="C229" t="s">
         <v>533</v>
       </c>
-      <c r="B229" t="s">
-        <v>477</v>
-      </c>
-      <c r="C229" t="s">
-        <v>534</v>
-      </c>
       <c r="D229">
-        <v>3512</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
+        <v>534</v>
+      </c>
+      <c r="B230" t="s">
+        <v>48</v>
+      </c>
+      <c r="C230" t="s">
         <v>535</v>
       </c>
-      <c r="B230" t="s">
-        <v>95</v>
-      </c>
-      <c r="C230" t="s">
-        <v>536</v>
-      </c>
       <c r="D230">
-        <v>3390</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
+        <v>536</v>
+      </c>
+      <c r="B231" t="s">
+        <v>113</v>
+      </c>
+      <c r="C231" t="s">
         <v>537</v>
       </c>
-      <c r="B231" t="s">
-        <v>48</v>
-      </c>
-      <c r="C231" t="s">
-        <v>538</v>
-      </c>
       <c r="D231">
-        <v>3737</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
+        <v>538</v>
+      </c>
+      <c r="B232" t="s">
+        <v>272</v>
+      </c>
+      <c r="C232" t="s">
         <v>539</v>
       </c>
-      <c r="B232" t="s">
-        <v>113</v>
-      </c>
-      <c r="C232" t="s">
-        <v>540</v>
-      </c>
       <c r="D232">
-        <v>3608</v>
+        <v>3805</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
+        <v>540</v>
+      </c>
+      <c r="B233" t="s">
+        <v>255</v>
+      </c>
+      <c r="C233" t="s">
         <v>541</v>
       </c>
-      <c r="B233" t="s">
-        <v>274</v>
-      </c>
-      <c r="C233" t="s">
-        <v>542</v>
-      </c>
       <c r="D233">
-        <v>3805</v>
+        <v>3638</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
+        <v>542</v>
+      </c>
+      <c r="B234" t="s">
+        <v>348</v>
+      </c>
+      <c r="C234" t="s">
         <v>543</v>
       </c>
-      <c r="B234" t="s">
-        <v>257</v>
-      </c>
-      <c r="C234" t="s">
-        <v>544</v>
-      </c>
       <c r="D234">
-        <v>3638</v>
+        <v>3409</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
+        <v>544</v>
+      </c>
+      <c r="B235" t="s">
+        <v>314</v>
+      </c>
+      <c r="C235" t="s">
         <v>545</v>
       </c>
-      <c r="B235" t="s">
-        <v>350</v>
-      </c>
-      <c r="C235" t="s">
-        <v>546</v>
-      </c>
       <c r="D235">
-        <v>3409</v>
+        <v>3831</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
+        <v>546</v>
+      </c>
+      <c r="B236" t="s">
         <v>547</v>
-      </c>
-      <c r="B236" t="s">
-        <v>316</v>
       </c>
       <c r="C236" t="s">
         <v>548</v>
       </c>
       <c r="D236">
-        <v>3831</v>
+        <v>3225</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
@@ -5967,265 +5961,265 @@
         <v>549</v>
       </c>
       <c r="B237" t="s">
+        <v>314</v>
+      </c>
+      <c r="C237" t="s">
         <v>550</v>
       </c>
-      <c r="C237" t="s">
-        <v>551</v>
-      </c>
       <c r="D237">
-        <v>3225</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
+        <v>551</v>
+      </c>
+      <c r="B238" t="s">
+        <v>474</v>
+      </c>
+      <c r="C238" t="s">
         <v>552</v>
       </c>
-      <c r="B238" t="s">
-        <v>316</v>
-      </c>
-      <c r="C238" t="s">
-        <v>553</v>
-      </c>
       <c r="D238">
-        <v>3825</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
+        <v>553</v>
+      </c>
+      <c r="B239" t="s">
+        <v>440</v>
+      </c>
+      <c r="C239" t="s">
         <v>554</v>
       </c>
-      <c r="B239" t="s">
-        <v>477</v>
-      </c>
-      <c r="C239" t="s">
-        <v>555</v>
-      </c>
       <c r="D239">
-        <v>3496</v>
+        <v>3073</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
+        <v>555</v>
+      </c>
+      <c r="B240" t="s">
+        <v>178</v>
+      </c>
+      <c r="C240" t="s">
         <v>556</v>
       </c>
-      <c r="B240" t="s">
-        <v>442</v>
-      </c>
-      <c r="C240" t="s">
-        <v>557</v>
-      </c>
       <c r="D240">
-        <v>3073</v>
+        <v>3121</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
+        <v>557</v>
+      </c>
+      <c r="B241" t="s">
+        <v>11</v>
+      </c>
+      <c r="C241" t="s">
         <v>558</v>
       </c>
-      <c r="B241" t="s">
-        <v>178</v>
-      </c>
-      <c r="C241" t="s">
-        <v>559</v>
-      </c>
       <c r="D241">
-        <v>3121</v>
+        <v>3431</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
+        <v>559</v>
+      </c>
+      <c r="B242" t="s">
+        <v>275</v>
+      </c>
+      <c r="C242" t="s">
         <v>560</v>
       </c>
-      <c r="B242" t="s">
-        <v>11</v>
-      </c>
-      <c r="C242" t="s">
-        <v>561</v>
-      </c>
       <c r="D242">
-        <v>3431</v>
+        <v>3134</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
+        <v>561</v>
+      </c>
+      <c r="B243" t="s">
+        <v>386</v>
+      </c>
+      <c r="C243" t="s">
         <v>562</v>
       </c>
-      <c r="B243" t="s">
-        <v>277</v>
-      </c>
-      <c r="C243" t="s">
-        <v>563</v>
-      </c>
       <c r="D243">
-        <v>3134</v>
+        <v>3549</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
+        <v>563</v>
+      </c>
+      <c r="B244" t="s">
+        <v>60</v>
+      </c>
+      <c r="C244" t="s">
         <v>564</v>
       </c>
-      <c r="B244" t="s">
-        <v>388</v>
-      </c>
-      <c r="C244" t="s">
-        <v>565</v>
-      </c>
       <c r="D244">
-        <v>3549</v>
+        <v>3561</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
+        <v>565</v>
+      </c>
+      <c r="B245" t="s">
+        <v>51</v>
+      </c>
+      <c r="C245" t="s">
         <v>566</v>
       </c>
-      <c r="B245" t="s">
-        <v>60</v>
-      </c>
-      <c r="C245" t="s">
-        <v>567</v>
-      </c>
       <c r="D245">
-        <v>3561</v>
+        <v>3330</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
+        <v>567</v>
+      </c>
+      <c r="B246" t="s">
+        <v>11</v>
+      </c>
+      <c r="C246" t="s">
         <v>568</v>
       </c>
-      <c r="B246" t="s">
-        <v>51</v>
-      </c>
-      <c r="C246" t="s">
-        <v>569</v>
-      </c>
       <c r="D246">
-        <v>3330</v>
+        <v>3434</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
+        <v>569</v>
+      </c>
+      <c r="B247" t="s">
+        <v>311</v>
+      </c>
+      <c r="C247" t="s">
         <v>570</v>
       </c>
-      <c r="B247" t="s">
-        <v>11</v>
-      </c>
-      <c r="C247" t="s">
-        <v>571</v>
-      </c>
       <c r="D247">
-        <v>3434</v>
+        <v>3939</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
+        <v>571</v>
+      </c>
+      <c r="B248" t="s">
+        <v>122</v>
+      </c>
+      <c r="C248" t="s">
         <v>572</v>
       </c>
-      <c r="B248" t="s">
-        <v>313</v>
-      </c>
-      <c r="C248" t="s">
-        <v>573</v>
-      </c>
       <c r="D248">
-        <v>3939</v>
+        <v>3847</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
+        <v>573</v>
+      </c>
+      <c r="B249" t="s">
+        <v>173</v>
+      </c>
+      <c r="C249" t="s">
         <v>574</v>
       </c>
-      <c r="B249" t="s">
-        <v>122</v>
-      </c>
-      <c r="C249" t="s">
-        <v>575</v>
-      </c>
       <c r="D249">
-        <v>3847</v>
+        <v>3178</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
+        <v>575</v>
+      </c>
+      <c r="B250" t="s">
+        <v>60</v>
+      </c>
+      <c r="C250" t="s">
         <v>576</v>
       </c>
-      <c r="B250" t="s">
-        <v>173</v>
-      </c>
-      <c r="C250" t="s">
-        <v>577</v>
-      </c>
       <c r="D250">
-        <v>3178</v>
+        <v>3612</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
+        <v>577</v>
+      </c>
+      <c r="B251" t="s">
+        <v>148</v>
+      </c>
+      <c r="C251" t="s">
         <v>578</v>
       </c>
-      <c r="B251" t="s">
-        <v>60</v>
-      </c>
-      <c r="C251" t="s">
-        <v>579</v>
-      </c>
       <c r="D251">
-        <v>3612</v>
+        <v>3685</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
+        <v>579</v>
+      </c>
+      <c r="B252" t="s">
+        <v>311</v>
+      </c>
+      <c r="C252" t="s">
         <v>580</v>
       </c>
-      <c r="B252" t="s">
-        <v>148</v>
-      </c>
-      <c r="C252" t="s">
-        <v>581</v>
-      </c>
       <c r="D252">
-        <v>3685</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
+        <v>581</v>
+      </c>
+      <c r="B253" t="s">
+        <v>122</v>
+      </c>
+      <c r="C253" t="s">
         <v>582</v>
       </c>
-      <c r="B253" t="s">
-        <v>313</v>
-      </c>
-      <c r="C253" t="s">
-        <v>583</v>
-      </c>
       <c r="D253">
-        <v>3941</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
+        <v>583</v>
+      </c>
+      <c r="B254" t="s">
+        <v>54</v>
+      </c>
+      <c r="C254" t="s">
         <v>584</v>
       </c>
-      <c r="B254" t="s">
-        <v>122</v>
-      </c>
-      <c r="C254" t="s">
-        <v>585</v>
-      </c>
       <c r="D254">
-        <v>3850</v>
+        <v>3925</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
+        <v>585</v>
+      </c>
+      <c r="B255" t="s">
         <v>586</v>
-      </c>
-      <c r="B255" t="s">
-        <v>54</v>
       </c>
       <c r="C255" t="s">
         <v>587</v>
       </c>
       <c r="D255">
-        <v>3925</v>
+        <v>3191</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
@@ -6233,1090 +6227,1076 @@
         <v>588</v>
       </c>
       <c r="B256" t="s">
+        <v>166</v>
+      </c>
+      <c r="C256" t="s">
         <v>589</v>
       </c>
-      <c r="C256" t="s">
-        <v>590</v>
-      </c>
       <c r="D256">
-        <v>3191</v>
+        <v>3533</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
+        <v>590</v>
+      </c>
+      <c r="B257" t="s">
+        <v>125</v>
+      </c>
+      <c r="C257" t="s">
         <v>591</v>
       </c>
-      <c r="B257" t="s">
-        <v>166</v>
-      </c>
-      <c r="C257" t="s">
-        <v>592</v>
-      </c>
       <c r="D257">
-        <v>3533</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
+        <v>592</v>
+      </c>
+      <c r="B258" t="s">
+        <v>130</v>
+      </c>
+      <c r="C258" t="s">
         <v>593</v>
       </c>
-      <c r="B258" t="s">
-        <v>125</v>
-      </c>
-      <c r="C258" t="s">
-        <v>594</v>
-      </c>
       <c r="D258">
-        <v>3517</v>
+        <v>3660</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
+        <v>594</v>
+      </c>
+      <c r="B259" t="s">
+        <v>87</v>
+      </c>
+      <c r="C259" t="s">
         <v>595</v>
       </c>
-      <c r="B259" t="s">
-        <v>130</v>
-      </c>
-      <c r="C259" t="s">
-        <v>596</v>
-      </c>
       <c r="D259">
-        <v>3660</v>
+        <v>3630</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
+        <v>596</v>
+      </c>
+      <c r="B260" t="s">
+        <v>311</v>
+      </c>
+      <c r="C260" t="s">
         <v>597</v>
       </c>
-      <c r="B260" t="s">
-        <v>87</v>
-      </c>
-      <c r="C260" t="s">
-        <v>598</v>
-      </c>
       <c r="D260">
-        <v>3630</v>
+        <v>3943</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
+        <v>598</v>
+      </c>
+      <c r="B261" t="s">
+        <v>104</v>
+      </c>
+      <c r="C261" t="s">
         <v>599</v>
       </c>
-      <c r="B261" t="s">
-        <v>313</v>
-      </c>
-      <c r="C261" t="s">
-        <v>600</v>
-      </c>
       <c r="D261">
-        <v>3943</v>
+        <v>3205</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
+        <v>600</v>
+      </c>
+      <c r="B262" t="s">
+        <v>151</v>
+      </c>
+      <c r="C262" t="s">
         <v>601</v>
       </c>
-      <c r="B262" t="s">
-        <v>104</v>
-      </c>
-      <c r="C262" t="s">
-        <v>602</v>
-      </c>
       <c r="D262">
-        <v>3205</v>
+        <v>3788</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
+        <v>602</v>
+      </c>
+      <c r="B263" t="s">
+        <v>139</v>
+      </c>
+      <c r="C263" t="s">
         <v>603</v>
       </c>
-      <c r="B263" t="s">
-        <v>151</v>
-      </c>
-      <c r="C263" t="s">
-        <v>604</v>
-      </c>
       <c r="D263">
-        <v>3788</v>
+        <v>3898</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B264" t="s">
         <v>139</v>
       </c>
       <c r="C264" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D264">
-        <v>3898</v>
+        <v>3888</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
+        <v>606</v>
+      </c>
+      <c r="B265" t="s">
+        <v>474</v>
+      </c>
+      <c r="C265" t="s">
         <v>607</v>
       </c>
-      <c r="B265" t="s">
-        <v>139</v>
-      </c>
-      <c r="C265" t="s">
-        <v>608</v>
-      </c>
       <c r="D265">
-        <v>3888</v>
+        <v>3490</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
+        <v>608</v>
+      </c>
+      <c r="B266" t="s">
+        <v>8</v>
+      </c>
+      <c r="C266" t="s">
         <v>609</v>
       </c>
-      <c r="B266" t="s">
-        <v>477</v>
-      </c>
-      <c r="C266" t="s">
-        <v>610</v>
-      </c>
       <c r="D266">
-        <v>3490</v>
+        <v>3810</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
+        <v>610</v>
+      </c>
+      <c r="B267" t="s">
+        <v>386</v>
+      </c>
+      <c r="C267" t="s">
         <v>611</v>
       </c>
-      <c r="B267" t="s">
-        <v>8</v>
-      </c>
-      <c r="C267" t="s">
-        <v>612</v>
-      </c>
       <c r="D267">
-        <v>3810</v>
+        <v>3597</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
+        <v>612</v>
+      </c>
+      <c r="B268" t="s">
+        <v>98</v>
+      </c>
+      <c r="C268" t="s">
         <v>613</v>
       </c>
-      <c r="B268" t="s">
-        <v>388</v>
-      </c>
-      <c r="C268" t="s">
-        <v>614</v>
-      </c>
       <c r="D268">
-        <v>3597</v>
+        <v>3269</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
+        <v>614</v>
+      </c>
+      <c r="B269" t="s">
+        <v>95</v>
+      </c>
+      <c r="C269" t="s">
         <v>615</v>
       </c>
-      <c r="B269" t="s">
-        <v>98</v>
-      </c>
-      <c r="C269" t="s">
-        <v>616</v>
-      </c>
       <c r="D269">
-        <v>3269</v>
+        <v>3488</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
+        <v>616</v>
+      </c>
+      <c r="B270" t="s">
+        <v>280</v>
+      </c>
+      <c r="C270" t="s">
         <v>617</v>
       </c>
-      <c r="B270" t="s">
-        <v>95</v>
-      </c>
-      <c r="C270" t="s">
-        <v>618</v>
-      </c>
       <c r="D270">
-        <v>3488</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
+        <v>618</v>
+      </c>
+      <c r="B271" t="s">
+        <v>427</v>
+      </c>
+      <c r="C271" t="s">
         <v>619</v>
       </c>
-      <c r="B271" t="s">
-        <v>282</v>
-      </c>
-      <c r="C271" t="s">
-        <v>620</v>
-      </c>
       <c r="D271">
-        <v>3171</v>
+        <v>3478</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>621</v>
+        <v>744</v>
       </c>
       <c r="B272" t="s">
-        <v>429</v>
+        <v>104</v>
       </c>
       <c r="C272" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D272">
-        <v>3478</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B273" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="C273" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D273">
-        <v>3182</v>
+        <v>3623</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B274" t="s">
-        <v>60</v>
+        <v>427</v>
       </c>
       <c r="C274" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D274">
-        <v>3623</v>
+        <v>3380</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B275" t="s">
-        <v>429</v>
+        <v>122</v>
       </c>
       <c r="C275" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D275">
-        <v>3380</v>
+        <v>3862</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B276" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="C276" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D276">
-        <v>3862</v>
+        <v>3429</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B277" t="s">
-        <v>133</v>
+        <v>379</v>
       </c>
       <c r="C277" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D277">
-        <v>3429</v>
+        <v>3284</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B278" t="s">
-        <v>381</v>
+        <v>263</v>
       </c>
       <c r="C278" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D278">
-        <v>3284</v>
+        <v>3223</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B279" t="s">
-        <v>265</v>
+        <v>229</v>
       </c>
       <c r="C279" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D279">
-        <v>3223</v>
+        <v>3305</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B280" t="s">
-        <v>231</v>
+        <v>457</v>
       </c>
       <c r="C280" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D280">
-        <v>3305</v>
+        <v>3181</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B281" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
       <c r="C281" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D281">
-        <v>3181</v>
+        <v>3072</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B282" t="s">
-        <v>442</v>
+        <v>130</v>
       </c>
       <c r="C282" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D282">
-        <v>3072</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B283" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C283" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D283">
-        <v>3521</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B284" t="s">
-        <v>125</v>
+        <v>258</v>
       </c>
       <c r="C284" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="D284">
-        <v>3575</v>
+        <v>3540</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B285" t="s">
-        <v>260</v>
+        <v>98</v>
       </c>
       <c r="C285" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D285">
-        <v>3540</v>
+        <v>3268</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B286" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="C286" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D286">
-        <v>3268</v>
+        <v>3621</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B287" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C287" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D287">
-        <v>3621</v>
+        <v>3962</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B288" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="C288" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D288">
-        <v>3962</v>
+        <v>3228</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B289" t="s">
-        <v>119</v>
+        <v>314</v>
       </c>
       <c r="C289" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D289">
-        <v>3228</v>
+        <v>3824</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B290" t="s">
-        <v>316</v>
+        <v>79</v>
       </c>
       <c r="C290" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="D290">
-        <v>3824</v>
+        <v>3844</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B291" t="s">
-        <v>79</v>
+        <v>255</v>
       </c>
       <c r="C291" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="D291">
-        <v>3844</v>
+        <v>3728</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B292" t="s">
-        <v>257</v>
+        <v>474</v>
       </c>
       <c r="C292" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D292">
-        <v>3728</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B293" t="s">
-        <v>477</v>
+        <v>34</v>
       </c>
       <c r="C293" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D293">
-        <v>3509</v>
+        <v>3133</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B294" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="C294" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D294">
-        <v>3133</v>
+        <v>3756</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B295" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="C295" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="D295">
-        <v>3756</v>
+        <v>3709</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B296" t="s">
-        <v>161</v>
+        <v>63</v>
       </c>
       <c r="C296" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D296">
-        <v>3709</v>
+        <v>3677</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B297" t="s">
-        <v>63</v>
+        <v>173</v>
       </c>
       <c r="C297" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="D297">
-        <v>3677</v>
+        <v>3152</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B298" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C298" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D298">
-        <v>3152</v>
+        <v>3799</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B299" t="s">
-        <v>151</v>
+        <v>95</v>
       </c>
       <c r="C299" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D299">
-        <v>3799</v>
+        <v>3393</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B300" t="s">
-        <v>95</v>
+        <v>314</v>
       </c>
       <c r="C300" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D300">
-        <v>3393</v>
+        <v>3820</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B301" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
       <c r="C301" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D301">
-        <v>3820</v>
+        <v>3113</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B302" t="s">
-        <v>295</v>
+        <v>125</v>
       </c>
       <c r="C302" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="D302">
-        <v>3113</v>
+        <v>3518</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
+        <v>681</v>
+      </c>
+      <c r="B303" t="s">
+        <v>682</v>
+      </c>
+      <c r="C303" t="s">
         <v>683</v>
       </c>
-      <c r="B303" t="s">
-        <v>125</v>
-      </c>
-      <c r="C303" t="s">
-        <v>684</v>
-      </c>
       <c r="D303">
-        <v>3518</v>
+        <v>3030</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
+        <v>684</v>
+      </c>
+      <c r="B304" t="s">
+        <v>474</v>
+      </c>
+      <c r="C304" t="s">
         <v>685</v>
       </c>
-      <c r="B304" t="s">
-        <v>686</v>
-      </c>
-      <c r="C304" t="s">
-        <v>687</v>
-      </c>
       <c r="D304">
-        <v>3030</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B305" t="s">
-        <v>477</v>
+        <v>63</v>
       </c>
       <c r="C305" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D305">
-        <v>3496</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B306" t="s">
-        <v>63</v>
+        <v>331</v>
       </c>
       <c r="C306" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D306">
-        <v>3733</v>
+        <v>3757</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B307" t="s">
-        <v>333</v>
+        <v>40</v>
       </c>
       <c r="C307" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D307">
-        <v>3757</v>
+        <v>3379</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B308" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="C308" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D308">
-        <v>3379</v>
+        <v>3016</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B309" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="C309" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D309">
-        <v>3016</v>
+        <v>3356</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
+        <v>696</v>
+      </c>
+      <c r="B310" t="s">
+        <v>697</v>
+      </c>
+      <c r="C310" t="s">
         <v>698</v>
       </c>
-      <c r="B310" t="s">
-        <v>31</v>
-      </c>
-      <c r="C310" t="s">
-        <v>699</v>
-      </c>
       <c r="D310">
-        <v>3356</v>
+        <v>3690</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
+        <v>699</v>
+      </c>
+      <c r="B311" t="s">
+        <v>364</v>
+      </c>
+      <c r="C311" t="s">
         <v>700</v>
       </c>
-      <c r="B311" t="s">
-        <v>701</v>
-      </c>
-      <c r="C311" t="s">
-        <v>702</v>
-      </c>
       <c r="D311">
-        <v>3690</v>
+        <v>3020</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B312" t="s">
-        <v>366</v>
+        <v>386</v>
       </c>
       <c r="C312" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D312">
-        <v>3020</v>
+        <v>3585</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B313" t="s">
-        <v>388</v>
+        <v>139</v>
       </c>
       <c r="C313" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="D313">
-        <v>3585</v>
+        <v>3896</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B314" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="C314" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D314">
-        <v>3896</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B315" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C315" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D315">
-        <v>3700</v>
+        <v>3691</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B316" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="C316" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D316">
-        <v>3691</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B317" t="s">
-        <v>125</v>
+        <v>682</v>
       </c>
       <c r="C317" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D317">
-        <v>3551</v>
+        <v>3029</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B318" t="s">
-        <v>686</v>
+        <v>87</v>
       </c>
       <c r="C318" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D318">
-        <v>3029</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B319" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="C319" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="D319">
-        <v>3616</v>
+        <v>3995</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B320" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="C320" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="D320">
-        <v>3995</v>
+        <v>3442</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B321" t="s">
-        <v>11</v>
+        <v>357</v>
       </c>
       <c r="C321" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D321">
-        <v>3442</v>
+        <v>3723</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B322" t="s">
-        <v>359</v>
+        <v>95</v>
       </c>
       <c r="C322" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="D322">
-        <v>3723</v>
+        <v>3485</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B323" t="s">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="C323" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="D323">
-        <v>3485</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B324" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="C324" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="D324">
-        <v>3527</v>
+        <v>3749</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B325" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C325" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D325">
-        <v>3749</v>
+        <v>3775</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B326" t="s">
         <v>151</v>
       </c>
       <c r="C326" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D326">
-        <v>3775</v>
+        <v>3797</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B327" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="C327" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D327">
-        <v>3797</v>
+        <v>3971</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B328" t="s">
-        <v>122</v>
+        <v>255</v>
       </c>
       <c r="C328" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D328">
-        <v>3971</v>
+        <v>3730</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B329" t="s">
-        <v>257</v>
+        <v>181</v>
       </c>
       <c r="C329" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D329">
-        <v>3730</v>
+        <v>3717</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B330" t="s">
-        <v>181</v>
+        <v>5</v>
       </c>
       <c r="C330" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D330">
-        <v>3717</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B331" t="s">
-        <v>5</v>
+        <v>229</v>
       </c>
       <c r="C331" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="D331">
-        <v>3250</v>
+        <v>3304</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B332" t="s">
-        <v>231</v>
+        <v>84</v>
       </c>
       <c r="C332" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D332">
-        <v>3304</v>
-      </c>
-    </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A333" t="s">
-        <v>745</v>
-      </c>
-      <c r="B333" t="s">
-        <v>84</v>
-      </c>
-      <c r="C333" t="s">
-        <v>746</v>
-      </c>
-      <c r="D333">
         <v>3960</v>
       </c>
     </row>

</xml_diff>